<commit_message>
Fix calculator and associated tests
</commit_message>
<xml_diff>
--- a/lib/utilities/analysis.xlsx
+++ b/lib/utilities/analysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dshendri/Turing/ModuleTwo/Projects/mo-money/lib/calculators/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dshendri/Turing/ModuleTwo/Projects/mo-money/lib/utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="1040" windowWidth="28800" windowHeight="20180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>Constants</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Variables</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Calculations</t>
   </si>
   <si>
@@ -56,12 +53,6 @@
     <t>Take Home Pay</t>
   </si>
   <si>
-    <t>// if city is San Francisco 17%, if city is New York than 23%</t>
-  </si>
-  <si>
-    <t>Denver</t>
-  </si>
-  <si>
     <t>annualSalary</t>
   </si>
   <si>
@@ -119,12 +110,6 @@
     <t>beer</t>
   </si>
   <si>
-    <t>company</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
     <t>workHoursInYear</t>
   </si>
   <si>
@@ -173,21 +158,9 @@
     <t>federalIncomeTaxRate</t>
   </si>
   <si>
-    <t>determineFederalIncomeTaxRate</t>
-  </si>
-  <si>
-    <t>determineCostOfLivingAdjustment</t>
-  </si>
-  <si>
     <t>totalBeer</t>
   </si>
   <si>
-    <t>&lt;  $91,150</t>
-  </si>
-  <si>
-    <t>&gt;= $91,150</t>
-  </si>
-  <si>
     <t>= Denver</t>
   </si>
   <si>
@@ -197,9 +170,6 @@
     <t>= New York City</t>
   </si>
   <si>
-    <t>iTriage</t>
-  </si>
-  <si>
     <t>weeksinYear</t>
   </si>
   <si>
@@ -210,6 +180,15 @@
   </si>
   <si>
     <t>totalIncomeAndBenefits</t>
+  </si>
+  <si>
+    <t>federalBaseTaxAmount</t>
+  </si>
+  <si>
+    <t>federalBaseTaxBracket</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -557,15 +536,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
@@ -576,74 +555,74 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E4" s="1">
-        <f>D36-D44</f>
-        <v>53246.5</v>
+        <f>$C$37-C45</f>
+        <v>58939.25</v>
       </c>
       <c r="F4" s="1">
         <f>E4/12</f>
-        <v>4437.208333333333</v>
+        <v>4911.604166666667</v>
       </c>
       <c r="G4" s="1">
         <f>E4/52</f>
-        <v>1023.9711538461538</v>
+        <v>1133.4471153846155</v>
       </c>
       <c r="H4" s="1">
         <f>E4/2080</f>
-        <v>25.599278846153847</v>
+        <v>28.336177884615385</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E5" s="3">
-        <f>E$4*$D$30</f>
-        <v>44194.595000000001</v>
-      </c>
-      <c r="F5" s="3">
-        <f>F$4*$D$30</f>
-        <v>3682.8829166666665</v>
-      </c>
-      <c r="G5" s="3">
-        <f>G$4*$D$30</f>
-        <v>849.89605769230764</v>
-      </c>
-      <c r="H5" s="3">
-        <f>H$4*$D$30</f>
-        <v>21.247401442307691</v>
+      <c r="E5" s="1">
+        <f>($C$37-D45)*D30</f>
+        <v>41620.424999999996</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ref="F5:F6" si="0">E5/12</f>
+        <v>3468.3687499999996</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G6" si="1">E5/52</f>
+        <v>800.39278846153843</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ref="H5:H6" si="2">E5/2080</f>
+        <v>20.009819711538459</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -651,31 +630,31 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>80000</v>
       </c>
-      <c r="E6" s="3">
-        <f>E$4*$E$30</f>
-        <v>40999.805</v>
-      </c>
-      <c r="F6" s="3">
-        <f>F$4*$E$30</f>
-        <v>3416.6504166666664</v>
-      </c>
-      <c r="G6" s="3">
-        <f>G$4*$E$30</f>
-        <v>788.45778846153848</v>
-      </c>
-      <c r="H6" s="3">
-        <f>H$4*$E$30</f>
-        <v>19.711444711538462</v>
+      <c r="E6" s="1">
+        <f>($C$37-E45)*E30</f>
+        <v>41673.5625</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>3472.796875</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>801.41466346153845</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>20.035366586538462</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>5000</v>
@@ -683,7 +662,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
         <v>7.0000000000000007E-2</v>
@@ -691,23 +670,23 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="7">
         <v>200</v>
@@ -715,386 +694,401 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="3">
+        <v>5183.75</v>
+      </c>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="3">
+        <v>37650</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="6">
+        <v>7.6499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1.4500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16">
-        <v>2080</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="6">
-        <v>7.6499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1.4500000000000001E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="6">
-        <v>9.4100000000000003E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>35</v>
       </c>
       <c r="C26" s="1">
         <v>8.5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C27" s="1">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1">
         <v>0.54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C29" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
       </c>
       <c r="D30" s="2">
-        <v>0.83</v>
+        <v>0.7</v>
       </c>
       <c r="E30" s="2">
-        <v>0.77</v>
-      </c>
-      <c r="F30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="6">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="D31" s="6">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.1338</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="1">
         <f>C6+C7</f>
         <v>85000</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
         <v>11</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="1">
+        <f>C33*C8</f>
+        <v>5950.0000000000009</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="1">
+        <f>IF(C9="Y",C15*C16*C26,0)</f>
+        <v>2040</v>
+      </c>
+      <c r="D35" t="s">
         <v>14</v>
       </c>
-      <c r="F32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="1">
-        <f>C32*C8</f>
-        <v>5950.0000000000009</v>
-      </c>
-      <c r="D33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
         <v>15</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="1">
-        <f>IF(C9="Y",C17*C18*C26,0)</f>
-        <v>2040</v>
-      </c>
-      <c r="D34" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="1">
+        <f>IF(C10="Y",C15*C16*C27,0)</f>
+        <v>2400</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
         <v>17</v>
       </c>
-      <c r="E34" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="1">
-        <f>IF(C10="Y",C17*C18*C27,0)</f>
-        <v>2040</v>
-      </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C36" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="1">
-        <f>SUM(C32:C35)</f>
-        <v>95030</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="1">
-        <f>($C$6+$C$7)*C22</f>
-        <v>21250</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C37" s="1">
+        <f>SUM(C33:C36)</f>
+        <v>95390</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="1">
+        <f>(C22+(((C6+C7)-C23)*C20))</f>
+        <v>17021.25</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="1">
-        <f>($C$6+$C$7)*C23</f>
-        <v>6502.5</v>
-      </c>
-      <c r="D39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C40" s="1">
         <f>($C$6+$C$7)*C24</f>
-        <v>1232.5</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>13</v>
+        <v>6502.5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C41" s="1">
         <f>($C$6+$C$7)*C25</f>
+        <v>1232.5</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="1">
+        <f>($C$6+$C$7)*C31</f>
         <v>7998.5</v>
       </c>
-      <c r="D41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="D42" s="1">
+        <f>($C$6+$C$7)*D31</f>
+        <v>7480</v>
+      </c>
+      <c r="E42" s="1">
+        <f>($C$6+$C$7)*E31</f>
+        <v>11373</v>
+      </c>
+      <c r="G42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="1">
+        <f>((C12*2)*C15*C16)*C28</f>
+        <v>1296</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="1">
+        <f>C11*C17</f>
+        <v>2400</v>
+      </c>
+      <c r="D44" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="1">
-        <f>(C12*2)*C17*C18</f>
-        <v>2400</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
         <v>24</v>
       </c>
-      <c r="E42" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="1">
-        <f>C11*C19</f>
-        <v>2400</v>
-      </c>
-      <c r="D43" t="s">
-        <v>26</v>
-      </c>
-      <c r="E43" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C44" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" s="1">
-        <f>SUM(C38:C43)</f>
-        <v>41783.5</v>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="1">
+        <f>SUM(C39:C44)</f>
+        <v>36450.75</v>
+      </c>
+      <c r="D45" s="1">
+        <f>SUM($C$39:$C$41)+D42+SUM($C$43:$C$44)</f>
+        <v>35932.25</v>
+      </c>
+      <c r="E45" s="1">
+        <f>SUM($C$39:$C$41)+E42+SUM($C$43:$C$44)</f>
+        <v>39825.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>